<commit_message>
add sales information and finalize
</commit_message>
<xml_diff>
--- a/public/form.xlsx
+++ b/public/form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus8\Documents\Project\rpx\client-service-agreement-form\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50152751-A56E-48F7-924C-4E9DB081C8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287C8EC4-E654-4C99-8F9D-7321E5D78CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="204">
   <si>
     <t>:</t>
   </si>
@@ -2417,12 +2417,6 @@
 Revisi : 2
 Halaman: 1 dari 1
 Tgl. Efektif :  06 Januari 2025</t>
-  </si>
-  <si>
-    <t>ET 3</t>
-  </si>
-  <si>
-    <t>TITIN SUSANTI</t>
   </si>
   <si>
     <t>WAPU</t>
@@ -20295,56 +20289,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>154082</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>182095</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>216041</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>135882</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Picture 66">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1662FEF2-57C7-45F9-93B4-4A99407DD7EC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9370920" y="22635882"/>
-          <a:ext cx="538209" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25435,8 +25379,8 @@
   </sheetPr>
   <dimension ref="B1:BF137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10:BF11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="AC105" sqref="AC105:AJ105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28430,13 +28374,13 @@
       <c r="AA15" s="78"/>
       <c r="AB15" s="76"/>
       <c r="AC15" s="76" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AD15" s="76"/>
       <c r="AE15" s="76"/>
       <c r="AF15" s="76"/>
       <c r="AG15" s="76" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AH15" s="76"/>
       <c r="AI15" s="76"/>
@@ -32165,9 +32109,7 @@
         <v>28</v>
       </c>
       <c r="W104" s="84"/>
-      <c r="X104" s="219" t="s">
-        <v>202</v>
-      </c>
+      <c r="X104" s="219"/>
       <c r="Y104" s="219"/>
       <c r="Z104" s="219"/>
       <c r="AA104" s="219"/>
@@ -32178,9 +32120,7 @@
       <c r="AD104" s="84"/>
       <c r="AF104" s="95"/>
       <c r="AG104" s="95"/>
-      <c r="AH104" s="95" t="s">
-        <v>203</v>
-      </c>
+      <c r="AH104" s="95"/>
       <c r="AI104" s="95"/>
       <c r="AJ104" s="95"/>
       <c r="AK104" s="95"/>

</xml_diff>